<commit_message>
Checking in case issue
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestGFO/GFO_MODEL.xlsx
+++ b/src/test/resources/TestDriver/TestGFO/GFO_MODEL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\TestGFO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\TestGFO\TestGFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AFB262-14C2-4F19-9D9C-251EB94063B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1395D6-33A4-470B-A918-C7BDC4D1321D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{BB024743-E9E1-4B1C-B6C6-502616E14BEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{BB024743-E9E1-4B1C-B6C6-502616E14BEF}"/>
   </bookViews>
   <sheets>
     <sheet name="PO" sheetId="13" r:id="rId1"/>
@@ -938,7 +938,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,7 +984,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,9 +1025,7 @@
   </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1084,8 +1082,8 @@
   </sheetPr>
   <dimension ref="A1:AH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,7 +2207,7 @@
         <v/>
       </c>
       <c r="D39" s="5" t="str">
-        <f>IF($B$7="","","Interest_Accrual")</f>
+        <f>IF($B$7="","","INTEREST_ACCRUAL")</f>
         <v/>
       </c>
       <c r="E39" s="39" t="str">
@@ -2235,7 +2233,7 @@
         <v/>
       </c>
       <c r="D40" s="5" t="str">
-        <f>IF($B$7="","","PayOff_InterestAdj")</f>
+        <f>IF($B$7="","","PAYOFF_INTERESTADJ")</f>
         <v/>
       </c>
       <c r="E40" s="39" t="str">
@@ -2261,7 +2259,7 @@
         <v/>
       </c>
       <c r="D41" s="5" t="str">
-        <f>IF($B$7="","","Capitalized_Interest")</f>
+        <f>IF($B$7="","","CAPITALIZED_INTEREST")</f>
         <v/>
       </c>
       <c r="E41" s="39" t="str">
@@ -2287,7 +2285,7 @@
         <v/>
       </c>
       <c r="D42" s="5" t="str">
-        <f>IF($B$7="","","Capitalized_Principal")</f>
+        <f>IF($B$7="","","CAPITALIZED_PRINCIPAL")</f>
         <v/>
       </c>
       <c r="E42" s="39" t="str">
@@ -2461,15 +2459,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SenttoValley xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">true</SenttoValley>
-    <TaxCatchAll xmlns="8580efd2-8184-469e-9c71-58014ca3276e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2719,21 +2714,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SenttoValley xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">true</SenttoValley>
+    <TaxCatchAll xmlns="8580efd2-8184-469e-9c71-58014ca3276e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A035CFEF-7BEE-4959-A36C-737CEF7227A3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44B57B0-B813-4FA9-94DC-13406D627308}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5473e3af-2a01-4602-ae48-e408a4bd7dae"/>
-    <ds:schemaRef ds:uri="8580efd2-8184-469e-9c71-58014ca3276e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2759,9 +2754,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44B57B0-B813-4FA9-94DC-13406D627308}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A035CFEF-7BEE-4959-A36C-737CEF7227A3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5473e3af-2a01-4602-ae48-e408a4bd7dae"/>
+    <ds:schemaRef ds:uri="8580efd2-8184-469e-9c71-58014ca3276e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating model of GFO
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestGFO/GFO_MODEL.xlsx
+++ b/src/test/resources/TestDriver/TestGFO/GFO_MODEL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\TestGFO\TestGFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7C6646-8A1C-49FA-8B63-A26639C7BEAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9FF054-9479-4D93-AD4E-6B6CCBF33128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{BB024743-E9E1-4B1C-B6C6-502616E14BEF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{BB024743-E9E1-4B1C-B6C6-502616E14BEF}"/>
   </bookViews>
   <sheets>
     <sheet name="PO" sheetId="13" r:id="rId1"/>
@@ -598,6 +598,9 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -607,9 +610,6 @@
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="8" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -939,8 +939,8 @@
   </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,10 +954,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>57</v>
       </c>
       <c r="C1" s="40" t="s">
@@ -999,10 +999,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>57</v>
       </c>
       <c r="C1" s="40" t="s">
@@ -1045,10 +1045,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>57</v>
       </c>
       <c r="C1" s="40" t="s">
@@ -1063,7 +1063,7 @@
       <c r="F1" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="46" t="s">
         <v>83</v>
       </c>
       <c r="H1" s="42" t="s">
@@ -1086,8 +1086,8 @@
   </sheetPr>
   <dimension ref="A1:AH42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D2" s="17">
         <f>$B$12</f>
-        <v>0</v>
+        <v>45688</v>
       </c>
       <c r="E2" s="17">
         <f>PO!B2</f>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="D3" s="17">
         <f>$B$12</f>
-        <v>0</v>
+        <v>45688</v>
       </c>
       <c r="E3" s="17">
         <f>PO!B2</f>
@@ -1203,7 +1203,7 @@
       </c>
       <c r="D4" s="17">
         <f>$B$12</f>
-        <v>0</v>
+        <v>45688</v>
       </c>
       <c r="E4" s="17">
         <f>PMT!B2</f>
@@ -1260,9 +1260,9 @@
       <c r="A11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="17" t="str">
+      <c r="B11" s="17">
         <f>IFERROR(EOMONTH(B12,-1),"")</f>
-        <v/>
+        <v>45657</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
@@ -1270,8 +1270,7 @@
         <v>25</v>
       </c>
       <c r="B12" s="17">
-        <f>EOD!A2</f>
-        <v>0</v>
+        <v>45688</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -1513,11 +1512,11 @@
         <v/>
       </c>
       <c r="F16" s="29" t="str">
-        <f>IF(B13&lt;&gt;"PIK","",IF(E2="","",E2))</f>
+        <f>IF(B13&lt;&gt;"PIK","",IF(E2=0,"",E2))</f>
         <v/>
       </c>
       <c r="G16" s="29" t="str">
-        <f>IF(B13&lt;&gt;"PIK","",IF(E4="","",E4))</f>
+        <f>IF(B13&lt;&gt;"PIK","",IF(E4=0,"",E4))</f>
         <v/>
       </c>
       <c r="H16" s="12" t="str">
@@ -1669,10 +1668,10 @@
         <v/>
       </c>
       <c r="F21" s="2"/>
-      <c r="G21" s="44" t="s">
+      <c r="G21" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="44"/>
+      <c r="H21" s="47"/>
       <c r="K21" s="5" t="s">
         <v>69</v>
       </c>
@@ -1680,10 +1679,10 @@
         <f>VLOOKUP($L$18,$A$35:$AC$35,Q33,FALSE)</f>
         <v/>
       </c>
-      <c r="O21" s="45" t="s">
+      <c r="O21" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="P21" s="45"/>
+      <c r="P21" s="48"/>
       <c r="Z21" s="2"/>
       <c r="AB21" s="2"/>
     </row>
@@ -1837,9 +1836,9 @@
       <c r="A30" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="17" t="str">
+      <c r="B30" s="17">
         <f>B11</f>
-        <v/>
+        <v>45657</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
@@ -1848,7 +1847,7 @@
       </c>
       <c r="B31" s="17">
         <f>B12</f>
-        <v>0</v>
+        <v>45688</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
@@ -2095,11 +2094,11 @@
         <v/>
       </c>
       <c r="K35" s="29" t="str">
-        <f>IF(B32&lt;&gt;"ACCRUAL","",IF(E4="","",E4))</f>
+        <f>IF(B32&lt;&gt;"ACCRUAL","",IF(E4=0,"",E4))</f>
         <v/>
       </c>
       <c r="L35" s="29" t="str">
-        <f>IF(B32&lt;&gt;"ACCRUAL","",IF(E2="","",E2))</f>
+        <f>IF(B32&lt;&gt;"ACCRUAL","",IF(E2=0,"",E2))</f>
         <v/>
       </c>
       <c r="M35" s="25" t="str">
@@ -2166,16 +2165,16 @@
     </row>
     <row r="36" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:34" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="46" t="s">
+      <c r="A37" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="46"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="46"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" s="38" t="s">
@@ -2334,10 +2333,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="44" t="s">
         <v>63</v>
       </c>
       <c r="C1" s="40" t="s">
@@ -2463,18 +2462,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SenttoValley xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">true</SenttoValley>
-    <TaxCatchAll xmlns="8580efd2-8184-469e-9c71-58014ca3276e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100034432B0E955F24AA0D41FCF01EE227F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d07f073a6955c7336ba87148cc0eb23a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5473e3af-2a01-4602-ae48-e408a4bd7dae" xmlns:ns3="4c6cca36-c6f2-4e5f-94ac-9f1b68c22470" xmlns:ns4="8580efd2-8184-469e-9c71-58014ca3276e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01e02218117e62831f8dc850c6006c19" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="5473e3af-2a01-4602-ae48-e408a4bd7dae"/>
@@ -2720,7 +2707,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2729,18 +2716,19 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A035CFEF-7BEE-4959-A36C-737CEF7227A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5473e3af-2a01-4602-ae48-e408a4bd7dae"/>
-    <ds:schemaRef ds:uri="8580efd2-8184-469e-9c71-58014ca3276e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SenttoValley xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">true</SenttoValley>
+    <TaxCatchAll xmlns="8580efd2-8184-469e-9c71-58014ca3276e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072BD484-720F-44FD-BEBA-CB48F121A92F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2760,10 +2748,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44B57B0-B813-4FA9-94DC-13406D627308}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A035CFEF-7BEE-4959-A36C-737CEF7227A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5473e3af-2a01-4602-ae48-e408a4bd7dae"/>
+    <ds:schemaRef ds:uri="8580efd2-8184-469e-9c71-58014ca3276e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
loading model after removing datedif
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestGFO/GFO_MODEL.xlsx
+++ b/src/test/resources/TestDriver/TestGFO/GFO_MODEL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\TestGFO\TestGFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9FF054-9479-4D93-AD4E-6B6CCBF33128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59ED073-AEAE-4338-B770-75EF5894F57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{BB024743-E9E1-4B1C-B6C6-502616E14BEF}"/>
   </bookViews>
@@ -517,7 +517,7 @@
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -534,9 +534,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -609,6 +606,10 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -954,22 +955,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="40" t="s">
         <v>78</v>
       </c>
     </row>
@@ -999,19 +1000,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="40" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1045,31 +1046,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="43" t="s">
+      <c r="E1" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="41" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1086,8 +1087,8 @@
   </sheetPr>
   <dimension ref="A1:AH42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,15 +1154,15 @@
         <f>EOD!E2</f>
         <v>0</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="16">
         <f>$B$12</f>
         <v>45688</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="16">
         <f>PO!B2</f>
         <v>0</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="32" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="6">
@@ -1177,15 +1178,15 @@
         <f>EOD!F2</f>
         <v>0</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="16">
         <f>$B$12</f>
         <v>45688</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <f>PO!B2</f>
         <v>0</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="32" t="s">
         <v>20</v>
       </c>
       <c r="G3" s="6">
@@ -1194,22 +1195,22 @@
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="16">
         <f>EOD!G2</f>
         <v>0</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="16">
         <f>$B$12</f>
         <v>45688</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <f>PMT!B2</f>
         <v>0</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="32" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="6">
@@ -1218,7 +1219,7 @@
       </c>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>53</v>
       </c>
       <c r="B5" s="6">
@@ -1227,7 +1228,7 @@
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="6">
@@ -1236,7 +1237,7 @@
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>60</v>
       </c>
       <c r="B7" s="6" t="str">
@@ -1245,7 +1246,7 @@
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>66</v>
       </c>
       <c r="B8" s="6">
@@ -1260,7 +1261,7 @@
       <c r="A11" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <f>IFERROR(EOMONTH(B12,-1),"")</f>
         <v>45657</v>
       </c>
@@ -1269,7 +1270,7 @@
       <c r="A12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>45688</v>
       </c>
       <c r="Q12" s="2"/>
@@ -1279,7 +1280,7 @@
       <c r="A13" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="24" t="str">
+      <c r="B13" s="23" t="str">
         <f>IF(B5="PIK",B5,"")</f>
         <v/>
       </c>
@@ -1491,19 +1492,19 @@
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="str">
+      <c r="A16" s="28" t="str">
         <f>IF(B13&lt;&gt;"PIK","",B7)</f>
         <v/>
       </c>
-      <c r="B16" s="34" t="str">
+      <c r="B16" s="33" t="str">
         <f>IF(B13&lt;&gt;"PIK","",B4)</f>
         <v/>
       </c>
-      <c r="C16" s="35" t="str">
+      <c r="C16" s="34" t="str">
         <f>IF(B13&lt;&gt;"PIK","",B6)</f>
         <v/>
       </c>
-      <c r="D16" s="28" t="str">
+      <c r="D16" s="27" t="str">
         <f>IF(B13&lt;&gt;"PIK","",B2)</f>
         <v/>
       </c>
@@ -1511,95 +1512,95 @@
         <f>IF(B13&lt;&gt;"PIK","",B3)</f>
         <v/>
       </c>
-      <c r="F16" s="29" t="str">
+      <c r="F16" s="28" t="str">
         <f>IF(B13&lt;&gt;"PIK","",IF(E2=0,"",E2))</f>
         <v/>
       </c>
-      <c r="G16" s="29" t="str">
+      <c r="G16" s="28" t="str">
         <f>IF(B13&lt;&gt;"PIK","",IF(E4=0,"",E4))</f>
         <v/>
       </c>
-      <c r="H16" s="12" t="str">
-        <f>IF(B13&lt;&gt;"PIK","",EDATE(B16,IF(DATEDIF(B16,$B$12,"m")=0,1,DATEDIF(B16,$B$12,"m"))))</f>
-        <v/>
-      </c>
-      <c r="I16" s="14" t="str">
+      <c r="H16" s="50" t="str">
+        <f>IF(B13&lt;&gt;"PIK","",EDATE(B16,IF( (YEAR(B31)-YEAR(B35))*12 + (MONTH(B31)-MONTH(B35)) - (DAY(B31) &lt; DAY(B35)) = 0,1, (YEAR(B31)-YEAR(B35))*12 + (MONTH(B31)-MONTH(B35)) - (DAY(B31) &lt; DAY(B35)))))</f>
+        <v/>
+      </c>
+      <c r="I16" s="13" t="str">
         <f>IF(B13&lt;&gt;"PIK","",IF(F16="","",DAY(F16-1)))</f>
         <v/>
       </c>
-      <c r="J16" s="14" t="str">
+      <c r="J16" s="13" t="str">
         <f>IF(B13&lt;&gt;"PIK","",IFERROR(DAY(G16-1),""))</f>
         <v/>
       </c>
-      <c r="K16" s="15" t="str">
+      <c r="K16" s="14" t="str">
         <f>IF(B13&lt;&gt;"PIK","",IFERROR(DAY($B$12)-J16,""))</f>
         <v/>
       </c>
-      <c r="L16" s="14" t="str">
+      <c r="L16" s="13" t="str">
         <f>IF(B13&lt;&gt;"PIK","",IF((H16-$B$11)-1&gt;31,($B$12-B16)+1,(H16-$B$11)-1))</f>
         <v/>
       </c>
-      <c r="M16" s="14" t="str">
+      <c r="M16" s="13" t="str">
         <f>IF(B13&lt;&gt;"PIK","",IF((H16-$B$11)-1&gt;31,"",IF(F16&lt;&gt;"",IF(I16&gt;L16,ABS(L16-I16)-1,0),$B$12-H16)+1))</f>
         <v/>
       </c>
-      <c r="N16" s="14" t="str">
+      <c r="N16" s="13" t="str">
         <f>IF(B13&lt;&gt;"PIK","",IFERROR(J16-L16,""))</f>
         <v/>
       </c>
-      <c r="O16" s="14" t="str">
+      <c r="O16" s="13" t="str">
         <f>IF(B13&lt;&gt;"PIK","",C16/36500)</f>
         <v/>
       </c>
-      <c r="P16" s="20" t="str">
+      <c r="P16" s="19" t="str">
         <f>IF(B13&lt;&gt;"PIK","",(O16*D16)*MIN(L16,I16))</f>
         <v/>
       </c>
-      <c r="Q16" s="21" t="str">
+      <c r="Q16" s="20" t="str">
         <f>IF(B13&lt;&gt;"PIK","",IF(OR(L16&gt;I16,(H16-$B$11)-1&gt;31),0,(E16+P16)))</f>
         <v/>
       </c>
-      <c r="R16" s="22" t="str">
+      <c r="R16" s="21" t="str">
         <f>IF(B13&lt;&gt;"PIK","",IF(L16&gt;I16,0,(D16+Q16)))</f>
         <v/>
       </c>
-      <c r="S16" s="31" t="str">
+      <c r="S16" s="30" t="str">
         <f>IF(B13&lt;&gt;"PIK","",G4)</f>
         <v/>
       </c>
-      <c r="T16" s="21" t="str">
+      <c r="T16" s="20" t="str">
         <f>IF(B13&lt;&gt;"PIK","",IFERROR(IF(G16="",(R16*O16)*M16,((R16*O16)*N16)+(((R16-S16)*O16)*K16)),))</f>
         <v/>
       </c>
-      <c r="U16" s="21" t="str">
+      <c r="U16" s="20" t="str">
         <f>IF(B13&lt;&gt;"PIK","",P16+T16)</f>
         <v/>
       </c>
-      <c r="V16" s="30" t="str">
+      <c r="V16" s="29" t="str">
         <f>IF(B13&lt;&gt;"PIK","",G2+G3)</f>
         <v/>
       </c>
-      <c r="W16" s="30" t="str">
+      <c r="W16" s="29" t="str">
         <f>IF(B13&lt;&gt;"PIK","",G3)</f>
         <v/>
       </c>
-      <c r="X16" s="23" t="str">
+      <c r="X16" s="22" t="str">
         <f>IF(B13&lt;&gt;"PIK","",0)</f>
         <v/>
       </c>
-      <c r="Y16" s="23" t="str">
+      <c r="Y16" s="22" t="str">
         <f>IF(B13&lt;&gt;"PIK","",W16+X16)</f>
         <v/>
       </c>
-      <c r="Z16" s="23" t="str">
+      <c r="Z16" s="22" t="str">
         <f>IF(B13&lt;&gt;"PIK","",IF(W16=0,0,-(E16+U16-Q16-W16)))</f>
         <v/>
       </c>
-      <c r="AA16" s="23" t="str">
+      <c r="AA16" s="22" t="str">
         <f>IF(B13&lt;&gt;"PIK","",D16-S16+Q16-(V16-W16))</f>
         <v/>
       </c>
-      <c r="AB16" s="23" t="str">
+      <c r="AB16" s="22" t="str">
         <f>IF(B13&lt;&gt;"PIK","",E16+U16-Q16-W16+Z16)</f>
         <v/>
       </c>
@@ -1624,14 +1625,14 @@
       <c r="C19" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="16" t="str">
+      <c r="D19" s="15" t="str">
         <f>VLOOKUP($D$18,$A$16:$AB$16,D14,FALSE)</f>
         <v/>
       </c>
       <c r="K19" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="L19" s="16" t="str">
+      <c r="L19" s="15" t="str">
         <f>VLOOKUP($L$18,$A$35:$AC$35,D33,FALSE)</f>
         <v/>
       </c>
@@ -1643,7 +1644,7 @@
       <c r="C20" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D20" s="16" t="str">
+      <c r="D20" s="15" t="str">
         <f>VLOOKUP($D$18,$A$16:$AB$16,E14,FALSE)</f>
         <v/>
       </c>
@@ -1651,7 +1652,7 @@
       <c r="K20" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="L20" s="16" t="str">
+      <c r="L20" s="15" t="str">
         <f>VLOOKUP($L$18,$A$35:$AC$35,E33,FALSE)</f>
         <v/>
       </c>
@@ -1668,10 +1669,10 @@
         <v/>
       </c>
       <c r="F21" s="2"/>
-      <c r="G21" s="47" t="s">
+      <c r="G21" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="47"/>
+      <c r="H21" s="46"/>
       <c r="K21" s="5" t="s">
         <v>69</v>
       </c>
@@ -1679,10 +1680,10 @@
         <f>VLOOKUP($L$18,$A$35:$AC$35,Q33,FALSE)</f>
         <v/>
       </c>
-      <c r="O21" s="48" t="s">
+      <c r="O21" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="P21" s="48"/>
+      <c r="P21" s="47"/>
       <c r="Z21" s="2"/>
       <c r="AB21" s="2"/>
     </row>
@@ -1690,7 +1691,7 @@
       <c r="C22" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="16" t="str">
+      <c r="D22" s="15" t="str">
         <f>IFERROR(-(VLOOKUP($D$18,$A$16:$AB$16,V14,FALSE)-VLOOKUP($D$18,$A$16:$AB$16,W14,FALSE)),"")</f>
         <v/>
       </c>
@@ -1703,7 +1704,7 @@
       <c r="K22" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="L22" s="16" t="str">
+      <c r="L22" s="15" t="str">
         <f>IFERROR(-(VLOOKUP($L$18,$A$35:$AC$35,U14,FALSE)-VLOOKUP($L$18,$A$35:$AC$35,AC14,FALSE)),"")</f>
         <v/>
       </c>
@@ -1720,7 +1721,7 @@
       <c r="C23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="16" t="str">
+      <c r="D23" s="15" t="str">
         <f>IFERROR(-(VLOOKUP($D$18,$A$16:$AB$16,W14,FALSE)),"")</f>
         <v/>
       </c>
@@ -1735,7 +1736,7 @@
       <c r="K23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="L23" s="16" t="str">
+      <c r="L23" s="15" t="str">
         <f>IFERROR(-VLOOKUP($L$18,$A$35:$AC$35,U33,FALSE),"")</f>
         <v/>
       </c>
@@ -1799,7 +1800,7 @@
       <c r="K25" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="L25" s="16" t="str">
+      <c r="L25" s="15" t="str">
         <f>IFERROR(-VLOOKUP($L$18,$A$35:$AC$35,S33,FALSE),"")</f>
         <v/>
       </c>
@@ -1827,7 +1828,7 @@
       <c r="C27" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="16" t="str">
+      <c r="D27" s="15" t="str">
         <f>IFERROR(-VLOOKUP($D$18,$A$16:$AB$16,S14,FALSE),"")</f>
         <v/>
       </c>
@@ -1836,7 +1837,7 @@
       <c r="A30" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="16">
         <f>B11</f>
         <v>45657</v>
       </c>
@@ -1845,7 +1846,7 @@
       <c r="A31" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="17">
+      <c r="B31" s="16">
         <f>B12</f>
         <v>45688</v>
       </c>
@@ -1854,7 +1855,7 @@
       <c r="A32" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="19" t="str">
+      <c r="B32" s="18" t="str">
         <f>IF(B5="ACCRUAL",B5,"")</f>
         <v/>
       </c>
@@ -1985,7 +1986,7 @@
       <c r="E34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="17" t="s">
         <v>41</v>
       </c>
       <c r="G34" s="1" t="s">
@@ -2053,19 +2054,19 @@
       </c>
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="str">
+      <c r="A35" s="28" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",B7)</f>
         <v/>
       </c>
-      <c r="B35" s="34" t="str">
+      <c r="B35" s="33" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",B4)</f>
         <v/>
       </c>
-      <c r="C35" s="35" t="str">
+      <c r="C35" s="34" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",B6)</f>
         <v/>
       </c>
-      <c r="D35" s="28" t="str">
+      <c r="D35" s="27" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",B2)</f>
         <v/>
       </c>
@@ -2073,90 +2074,90 @@
         <f>IF(B32&lt;&gt;"ACCRUAL","",B3)</f>
         <v/>
       </c>
-      <c r="F35" s="13" t="str">
+      <c r="F35" s="12" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",DAY($B$31))</f>
         <v/>
       </c>
-      <c r="G35" s="14" t="str">
+      <c r="G35" s="13" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",IF(L35="",0,(L35-$B$30)-1))</f>
         <v/>
       </c>
-      <c r="H35" s="14" t="str">
+      <c r="H35" s="13" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",IF(K35="",0,(K35-$B$30)-1))</f>
         <v/>
       </c>
-      <c r="I35" s="14" t="str">
-        <f>IF(B32&lt;&gt;"ACCRUAL","",IF(DATEDIF(B35,$B$31,"m")=0,$B$31-B35+1,0))</f>
-        <v/>
-      </c>
-      <c r="J35" s="14" t="str">
+      <c r="I35" s="6" t="str">
+        <f>IF(B32&lt;&gt;"ACCRUAL","",IF( (YEAR(B31)-YEAR(B35))*12 + (MONTH(B31)-MONTH(B35)) - (DAY(B31) &lt; DAY(B35)) = 0,$B$31-B35+1,0))</f>
+        <v/>
+      </c>
+      <c r="J35" s="13" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",C35/36500)</f>
         <v/>
       </c>
-      <c r="K35" s="29" t="str">
+      <c r="K35" s="28" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",IF(E4=0,"",E4))</f>
         <v/>
       </c>
-      <c r="L35" s="29" t="str">
+      <c r="L35" s="28" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",IF(E2=0,"",E2))</f>
         <v/>
       </c>
-      <c r="M35" s="25" t="str">
-        <f>IF(B32&lt;&gt;"ACCRUAL","",IF(AND(L35="",K35="",DATEDIF(B35,$B$31,"m")&lt;&gt;0),((J35-S35)*D35)*F35,0))</f>
-        <v/>
-      </c>
-      <c r="N35" s="26" t="str">
+      <c r="M35" s="24" t="str">
+        <f>IF(B32&lt;&gt;"ACCRUAL","",IF(AND(L35="",K35="", (YEAR(B31)-YEAR(B35))*12 + (MONTH(B31)-MONTH(B35)) - (DAY(B31) &lt; DAY(B35))&lt;&gt;0),((J35-S35)*D35)*F35,0))</f>
+        <v/>
+      </c>
+      <c r="N35" s="25" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",((J35*D35)*G35))</f>
         <v/>
       </c>
-      <c r="O35" s="26" t="str">
+      <c r="O35" s="25" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",IF(K35="",0,((D35*J35)*H35)+(((D35-S35)*J35)*(F35-H35))))</f>
         <v/>
       </c>
-      <c r="P35" s="26" t="str">
-        <f>IF(B32&lt;&gt;"ACCRUAL","",IF(DATEDIF(B35,$B$31,"m")=0,(D35*J35)*I35,0))</f>
-        <v/>
-      </c>
-      <c r="Q35" s="26" t="str">
+      <c r="P35" s="49" t="str">
+        <f>IF(B32&lt;&gt;"ACCRUAL","",IF( (YEAR(B31)-YEAR(B35))*12 + (MONTH(B31)-MONTH(B35)) - (DAY(B31) &lt; DAY(B35)) = 0,(D35*J35)*I35,0))</f>
+        <v/>
+      </c>
+      <c r="Q35" s="25" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",M35+N35+O35+P35)</f>
         <v/>
       </c>
-      <c r="R35" s="25">
+      <c r="R35" s="24">
         <v>0</v>
       </c>
-      <c r="S35" s="36" t="str">
+      <c r="S35" s="35" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",G4)</f>
         <v/>
       </c>
-      <c r="T35" s="37" t="str">
+      <c r="T35" s="36" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",G2+G3)</f>
         <v/>
       </c>
-      <c r="U35" s="37" t="str">
+      <c r="U35" s="36" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",G3)</f>
         <v/>
       </c>
-      <c r="V35" s="27" t="str">
+      <c r="V35" s="26" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",0)</f>
         <v/>
       </c>
-      <c r="W35" s="27" t="str">
+      <c r="W35" s="26" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",U35+V35)</f>
         <v/>
       </c>
-      <c r="X35" s="27" t="str">
+      <c r="X35" s="26" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",IF(W35=0,0,-(E35+Q35-W35)))</f>
         <v/>
       </c>
-      <c r="Y35" s="27" t="str">
+      <c r="Y35" s="26" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",X35+Q35)</f>
         <v/>
       </c>
-      <c r="Z35" s="27" t="str">
+      <c r="Z35" s="26" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",D35-S35-(T35-U35))</f>
         <v/>
       </c>
-      <c r="AA35" s="27" t="str">
+      <c r="AA35" s="26" t="str">
         <f>IF(B32&lt;&gt;"ACCRUAL","",E35+Q35-W35+X35)</f>
         <v/>
       </c>
@@ -2165,43 +2166,43 @@
     </row>
     <row r="36" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="1:34" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="49" t="s">
+      <c r="A37" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="49"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="48"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="38" t="s">
+      <c r="C38" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="E38" s="38" t="s">
+      <c r="E38" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="F38" s="38" t="s">
+      <c r="F38" s="37" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="str">
+      <c r="A39" s="16" t="str">
         <f>IF($B$7="","",$B$12)</f>
         <v/>
       </c>
-      <c r="B39" s="17" t="str">
+      <c r="B39" s="16" t="str">
         <f>IF($B$7="","",$A$39)</f>
         <v/>
       </c>
@@ -2213,7 +2214,7 @@
         <f>IF($B$7="","","INTEREST_ACCRUAL")</f>
         <v/>
       </c>
-      <c r="E39" s="39" t="str">
+      <c r="E39" s="38" t="str">
         <f>IF($B$7="","",IF(B5="PIK",ROUND(D21,4),ROUND(L21,4)))</f>
         <v/>
       </c>
@@ -2223,11 +2224,11 @@
       </c>
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="str">
+      <c r="A40" s="16" t="str">
         <f t="shared" ref="A40:A42" si="2">IF($B$7="","",$B$12)</f>
         <v/>
       </c>
-      <c r="B40" s="17" t="str">
+      <c r="B40" s="16" t="str">
         <f t="shared" ref="B40:B42" si="3">IF($B$7="","",$A$39)</f>
         <v/>
       </c>
@@ -2239,7 +2240,7 @@
         <f>IF($B$7="","","PAYOFF_INTERESTADJ")</f>
         <v/>
       </c>
-      <c r="E40" s="39" t="str">
+      <c r="E40" s="38" t="str">
         <f>IF($B$7="","",IF(B5="PIK",ROUND(D24,4),ROUND(L24,4)))</f>
         <v/>
       </c>
@@ -2249,11 +2250,11 @@
       </c>
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="str">
+      <c r="A41" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="B41" s="17" t="str">
+      <c r="B41" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -2265,7 +2266,7 @@
         <f>IF($B$7="","","CAPITALIZED_INTEREST")</f>
         <v/>
       </c>
-      <c r="E41" s="39" t="str">
+      <c r="E41" s="38" t="str">
         <f>IF($B$7="","",IF(B5="PIK",ROUND(D25,4),0))</f>
         <v/>
       </c>
@@ -2275,11 +2276,11 @@
       </c>
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="str">
+      <c r="A42" s="16" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="B42" s="17" t="str">
+      <c r="B42" s="16" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
@@ -2291,7 +2292,7 @@
         <f>IF($B$7="","","CAPITALIZED_PRINCIPAL")</f>
         <v/>
       </c>
-      <c r="E42" s="39" t="str">
+      <c r="E42" s="38" t="str">
         <f>IF($B$7="","",IF(B5="PIK",ROUND(D26,4),0))</f>
         <v/>
       </c>
@@ -2333,22 +2334,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="39" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2708,15 +2709,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SenttoValley xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">true</SenttoValley>
@@ -2726,6 +2718,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2749,14 +2750,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44B57B0-B813-4FA9-94DC-13406D627308}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A035CFEF-7BEE-4959-A36C-737CEF7227A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2765,4 +2758,12 @@
     <ds:schemaRef ds:uri="8580efd2-8184-469e-9c71-58014ca3276e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44B57B0-B813-4FA9-94DC-13406D627308}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Replacing, Datedif,Edate and Eomonth formulas
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestGFO/GFO_MODEL.xlsx
+++ b/src/test/resources/TestDriver/TestGFO/GFO_MODEL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\TestGFO\TestGFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555A7D8D-D04B-4F1B-921C-A346FAE8FBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF62CC2-F86B-404F-B168-839145CDA170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{BB024743-E9E1-4B1C-B6C6-502616E14BEF}"/>
   </bookViews>
@@ -1088,7 +1088,7 @@
   <dimension ref="A1:AH42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,6 +1262,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="16">
+        <f>DATE(YEAR(B12), MONTH(B12), 0)</f>
         <v>45657</v>
       </c>
     </row>
@@ -1520,7 +1521,16 @@
         <v/>
       </c>
       <c r="H16" s="47" t="str">
-        <f>IF(B13&lt;&gt;"PIK","",EDATE(B16,IF( (YEAR(B31)-YEAR(B35))*12 + (MONTH(B31)-MONTH(B35)) - (DAY(B31) &lt; DAY(B35)) = 0,1, (YEAR(B31)-YEAR(B35))*12 + (MONTH(B31)-MONTH(B35)) - (DAY(B31) &lt; DAY(B35)))))</f>
+        <f>IF(B13&lt;&gt;"PIK","",DATE(
+YEAR(B16),
+MONTH(B16)+
+IF(
+((YEAR($B$12)-YEAR(B16))*12+(MONTH($B$12)-MONTH(B16))---(DAY($B$12)&lt;DAY(B16)))=0,
+1,
+(YEAR($B$12)-YEAR(B16))*12+(MONTH($B$12)-MONTH(B16))---(DAY($B$12)&lt;DAY(B16))
+),
+DAY(B16)
+))</f>
         <v/>
       </c>
       <c r="I16" s="13" t="str">
@@ -2086,7 +2096,11 @@
         <v/>
       </c>
       <c r="I35" s="6" t="str">
-        <f>IF(B32&lt;&gt;"ACCRUAL","",IF( (YEAR(B31)-YEAR(B35))*12 + (MONTH(B31)-MONTH(B35)) - (DAY(B31) &lt; DAY(B35)) = 0,$B$31-B35+1,0))</f>
+        <f>IF(B32&lt;&gt;"ACCRUAL","",IF(
+((YEAR($B$31)-YEAR(B35))*12+(MONTH($B$31)-MONTH(B35))---(DAY($B$31)&lt;DAY(B35)))=0,
+$B$31-B35+1,
+0
+))</f>
         <v/>
       </c>
       <c r="J35" s="13" t="str">
@@ -2102,7 +2116,15 @@
         <v/>
       </c>
       <c r="M35" s="24" t="str">
-        <f>IF(B32&lt;&gt;"ACCRUAL","",IF(AND(L35="",K35="", (YEAR(B31)-YEAR(B35))*12 + (MONTH(B31)-MONTH(B35)) - (DAY(B31) &lt; DAY(B35))&lt;&gt;0),((J35-S35)*D35)*F35,0))</f>
+        <f>IF(B32&lt;&gt;"ACCRUAL","",IF(
+AND(
+L35="",
+K35="",
+((YEAR($B$31)-YEAR(B35))*12+(MONTH($B$31)-MONTH(B35))---(DAY($B$31)&lt;DAY(B35)))&lt;&gt;0
+),
+((J35-S35)*D35)*F35,
+0
+))</f>
         <v/>
       </c>
       <c r="N35" s="25" t="str">
@@ -2114,7 +2136,11 @@
         <v/>
       </c>
       <c r="P35" s="46" t="str">
-        <f>IF(B32&lt;&gt;"ACCRUAL","",IF( (YEAR(B31)-YEAR(B35))*12 + (MONTH(B31)-MONTH(B35)) - (DAY(B31) &lt; DAY(B35)) = 0,(D35*J35)*I35,0))</f>
+        <f>IF(B32&lt;&gt;"ACCRUAL","",IF(
+((YEAR($B$31)-YEAR(B35))*12+(MONTH($B$31)-MONTH(B35))---(DAY($B$31)&lt;DAY(B35)))=0,
+(D35*J35)*I35,
+0
+))</f>
         <v/>
       </c>
       <c r="Q35" s="25" t="str">
@@ -2462,27 +2488,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SenttoValley xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">true</SenttoValley>
-    <TaxCatchAll xmlns="8580efd2-8184-469e-9c71-58014ca3276e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100034432B0E955F24AA0D41FCF01EE227F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d07f073a6955c7336ba87148cc0eb23a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5473e3af-2a01-4602-ae48-e408a4bd7dae" xmlns:ns3="4c6cca36-c6f2-4e5f-94ac-9f1b68c22470" xmlns:ns4="8580efd2-8184-469e-9c71-58014ca3276e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01e02218117e62831f8dc850c6006c19" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="5473e3af-2a01-4602-ae48-e408a4bd7dae"/>
@@ -2728,26 +2733,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A035CFEF-7BEE-4959-A36C-737CEF7227A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5473e3af-2a01-4602-ae48-e408a4bd7dae"/>
-    <ds:schemaRef ds:uri="8580efd2-8184-469e-9c71-58014ca3276e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44B57B0-B813-4FA9-94DC-13406D627308}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SenttoValley xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">true</SenttoValley>
+    <TaxCatchAll xmlns="8580efd2-8184-469e-9c71-58014ca3276e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072BD484-720F-44FD-BEBA-CB48F121A92F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2765,4 +2772,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44B57B0-B813-4FA9-94DC-13406D627308}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A035CFEF-7BEE-4959-A36C-737CEF7227A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5473e3af-2a01-4602-ae48-e408a4bd7dae"/>
+    <ds:schemaRef ds:uri="8580efd2-8184-469e-9c71-58014ca3276e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
checkin in updated model
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDriver/TestGFO/GFO_MODEL.xlsx
+++ b/src/test/resources/TestDriver/TestGFO/GFO_MODEL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arahmed\OneDrive - SS&amp;C Technologies, Inc\Desktop\Pers\TestGFO\TestGFO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF62CC2-F86B-404F-B168-839145CDA170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9451E6C-58B9-4653-8135-7FC6012EC822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{BB024743-E9E1-4B1C-B6C6-502616E14BEF}"/>
   </bookViews>
@@ -1088,7 +1088,7 @@
   <dimension ref="A1:AH42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1158,9 +1158,9 @@
         <f>$B$12</f>
         <v>45688</v>
       </c>
-      <c r="E2" s="16">
-        <f>PO!B2</f>
-        <v>0</v>
+      <c r="E2" s="16" t="str">
+        <f>IF(PO!E2="","",PO!B2)</f>
+        <v/>
       </c>
       <c r="F2" s="32" t="s">
         <v>19</v>
@@ -1182,9 +1182,9 @@
         <f>$B$12</f>
         <v>45688</v>
       </c>
-      <c r="E3" s="16">
-        <f>PO!B2</f>
-        <v>0</v>
+      <c r="E3" s="16" t="str">
+        <f>IF(PO!E2="","",PO!B2)</f>
+        <v/>
       </c>
       <c r="F3" s="32" t="s">
         <v>20</v>
@@ -1206,9 +1206,9 @@
         <f>$B$12</f>
         <v>45688</v>
       </c>
-      <c r="E4" s="16">
-        <f>PMT!B2</f>
-        <v>0</v>
+      <c r="E4" s="16" t="str">
+        <f>IF(PMT!E2="","",PMT!B2)</f>
+        <v/>
       </c>
       <c r="F4" s="32" t="s">
         <v>21</v>
@@ -2488,6 +2488,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SenttoValley xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">true</SenttoValley>
+    <TaxCatchAll xmlns="8580efd2-8184-469e-9c71-58014ca3276e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100034432B0E955F24AA0D41FCF01EE227F" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d07f073a6955c7336ba87148cc0eb23a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5473e3af-2a01-4602-ae48-e408a4bd7dae" xmlns:ns3="4c6cca36-c6f2-4e5f-94ac-9f1b68c22470" xmlns:ns4="8580efd2-8184-469e-9c71-58014ca3276e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01e02218117e62831f8dc850c6006c19" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="5473e3af-2a01-4602-ae48-e408a4bd7dae"/>
@@ -2733,28 +2754,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A035CFEF-7BEE-4959-A36C-737CEF7227A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5473e3af-2a01-4602-ae48-e408a4bd7dae"/>
+    <ds:schemaRef ds:uri="8580efd2-8184-469e-9c71-58014ca3276e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SenttoValley xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">true</SenttoValley>
-    <TaxCatchAll xmlns="8580efd2-8184-469e-9c71-58014ca3276e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5473e3af-2a01-4602-ae48-e408a4bd7dae">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44B57B0-B813-4FA9-94DC-13406D627308}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072BD484-720F-44FD-BEBA-CB48F121A92F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2772,23 +2791,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B44B57B0-B813-4FA9-94DC-13406D627308}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A035CFEF-7BEE-4959-A36C-737CEF7227A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5473e3af-2a01-4602-ae48-e408a4bd7dae"/>
-    <ds:schemaRef ds:uri="8580efd2-8184-469e-9c71-58014ca3276e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>